<commit_message>
finish import defects to tickets
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\VUE\Shlomi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3D9CCA-DF8D-4A11-8793-5724A6F34289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E399CE24-0D21-474F-B7FF-20DD4FD60739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{947F1416-3FCC-491B-9E78-B0402478432D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>משהו חדש שלי</t>
   </si>
 </sst>
 </file>
@@ -472,9 +475,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C85011-7339-479A-9EF5-B3F43AA93FEC}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -508,13 +513,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>8458</v>
@@ -522,10 +527,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -536,10 +541,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -550,10 +555,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -564,10 +569,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -578,10 +583,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -592,10 +597,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -606,10 +611,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -620,10 +625,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -634,24 +639,24 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>8459</v>
+        <v>8458</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -662,13 +667,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>8459</v>
@@ -676,10 +681,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -690,10 +695,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -704,10 +709,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -718,10 +723,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -732,10 +737,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -746,10 +751,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -760,10 +765,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -774,10 +779,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -788,10 +793,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -802,10 +807,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>9</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -816,27 +821,27 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>8460</v>
+        <v>8459</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <v>8460</v>
@@ -844,10 +849,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -858,10 +863,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -872,10 +877,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -886,10 +891,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -900,10 +905,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -914,27 +919,27 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>8461</v>
+        <v>8460</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>8461</v>
@@ -942,15 +947,29 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>8461</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>26</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
         <v>8461</v>
       </c>
     </row>

</xml_diff>